<commit_message>
change aoutput filenames to clarify from CBEP data
Also changed author in YAML header to include CBEP references.
</commit_message>
<xml_diff>
--- a/Analysis/summarystats table cleaned up.xlsx
+++ b/Analysis/summarystats table cleaned up.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Dropbox\Work\CBEP_OA\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Desktop\Current Projects\State of the Bay 2020\Data\CBEP_OA\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -87,7 +87,7 @@
     </r>
   </si>
   <si>
-    <t>Aragonite</t>
+    <t>Omega Aragonite</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>